<commit_message>
Model accommodating both reading from files and from nasa, some changes to objects' methods and tweaks in visualizer
</commit_message>
<xml_diff>
--- a/src/main/resources/model/initial_stats.xlsx
+++ b/src/main/resources/model/initial_stats.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marcell/Documents/*School/Year 1/Semester 2/Project 1-2/Phase 2/Graphics/src/main/resources/model/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marcell/Desktop/copy/src/main/resources/model/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7CF1EE8-334E-014B-AFCD-9B8979E6A1C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2695038-7D5E-604F-8189-AFA3F1BF8CE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17140" yWindow="860" windowWidth="16460" windowHeight="18940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7380" yWindow="1380" windowWidth="16460" windowHeight="18940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="initial" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Sun</t>
   </si>
@@ -66,9 +66,6 @@
   </si>
   <si>
     <t>Uranus</t>
-  </si>
-  <si>
-    <t>m (kg)</t>
   </si>
   <si>
     <t>Mass of the spaceship: 50000 kg</t>
@@ -531,7 +528,7 @@
   <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="H1" sqref="H1:H1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -547,26 +544,24 @@
   <sheetData>
     <row r="1" spans="1:8" s="3" customFormat="1" ht="17" x14ac:dyDescent="0.25">
       <c r="B1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="G1" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>10</v>
-      </c>
+      <c r="H1" s="4"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
@@ -590,10 +585,7 @@
       <c r="G2" s="1">
         <v>0</v>
       </c>
-      <c r="H2" s="1">
-        <f>1.9885*10^30</f>
-        <v>1.9885E+30</v>
-      </c>
+      <c r="H2" s="1"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
@@ -617,10 +609,7 @@
       <c r="G3" s="1">
         <v>6.2169537433413602</v>
       </c>
-      <c r="H3" s="1">
-        <f>3.302*10^23</f>
-        <v>3.3019999999999999E+23</v>
-      </c>
+      <c r="H3" s="1"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
@@ -644,14 +633,11 @@
       <c r="G4" s="1">
         <v>1.8406173527918801</v>
       </c>
-      <c r="H4" s="1">
-        <f>48.685 *10^23</f>
-        <v>4.8684999999999998E+24</v>
-      </c>
+      <c r="H4" s="1"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B5" s="2">
         <v>-148186906.89364201</v>
@@ -671,10 +657,7 @@
       <c r="G5" s="1">
         <v>1.7097427740129199E-3</v>
       </c>
-      <c r="H5" s="1">
-        <f>5.97219*10^24</f>
-        <v>5.9721900000000004E+24</v>
-      </c>
+      <c r="H5" s="1"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
@@ -698,10 +681,7 @@
       <c r="G6" s="1">
         <v>-1.16103535014229E-2</v>
       </c>
-      <c r="H6" s="1">
-        <f>7.349 *10^22</f>
-        <v>7.3489999999999999E+22</v>
-      </c>
+      <c r="H6" s="1"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
@@ -725,10 +705,7 @@
       <c r="G7" s="1">
         <v>0.15233192820053101</v>
       </c>
-      <c r="H7" s="1">
-        <f>6.4171*10^23</f>
-        <v>6.417099999999999E+23</v>
-      </c>
+      <c r="H7" s="1"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
@@ -752,10 +729,7 @@
       <c r="G8" s="1">
         <v>5.2211812693920799E-2</v>
       </c>
-      <c r="H8" s="2">
-        <f>189818722*10^19</f>
-        <v>1.89818722E+27</v>
-      </c>
+      <c r="H8" s="2"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
@@ -779,10 +753,7 @@
       <c r="G9" s="1">
         <v>-0.32074537696973199</v>
       </c>
-      <c r="H9" s="2">
-        <f>5.6834*10^26</f>
-        <v>5.6834000000000003E+26</v>
-      </c>
+      <c r="H9" s="2"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
@@ -806,10 +777,7 @@
       <c r="G10" s="1">
         <v>-2.2513098617476102</v>
       </c>
-      <c r="H10" s="2">
-        <f>13455.3*10^19</f>
-        <v>1.3455299999999999E+23</v>
-      </c>
+      <c r="H10" s="2"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
@@ -833,10 +801,7 @@
       <c r="G11" s="1">
         <v>-0.122638125365954</v>
       </c>
-      <c r="H11" s="2">
-        <f>102.409*10^24</f>
-        <v>1.0240900000000001E+26</v>
-      </c>
+      <c r="H11" s="2"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
@@ -860,19 +825,16 @@
       <c r="G12" s="1">
         <v>8.2119033640306302E-2</v>
       </c>
-      <c r="H12" s="2">
-        <f>86.813*10^24</f>
-        <v>8.6813E+25</v>
-      </c>
+      <c r="H12" s="2"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>